<commit_message>
pruebas de calculo sistemas de comiciones
</commit_message>
<xml_diff>
--- a/Contabilidad/plantilla.xlsx
+++ b/Contabilidad/plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Documentos\Proyectos\SQLServer-MySQL\Contabilidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F589C3-CDB5-40AD-B3A0-22130FA2E008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D1DDBB-B774-4748-AA4B-6AE5AB59A47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F77BE47C-2336-4147-857C-86466C8AA549}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="26">
   <si>
     <t>Personal</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>QUITO (UIO)</t>
+  </si>
+  <si>
+    <t>Tasa de C.</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -555,12 +558,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -607,80 +608,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -709,6 +657,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1047,70 +1067,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A56219-B1D8-4D34-BF55-7546737A25D9}">
   <dimension ref="A2:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="35" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="37" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="35" t="s">
+      <c r="G3" s="75"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="40" t="s">
+      <c r="J3" s="61"/>
+      <c r="K3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="35" t="s">
+      <c r="L3" s="60"/>
+      <c r="M3" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="35"/>
+      <c r="N3" s="61"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1146,22 +1166,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="45"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="72"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1170,450 +1190,450 @@
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="23">
-        <v>0</v>
-      </c>
-      <c r="D6" s="26">
-        <v>0</v>
-      </c>
-      <c r="E6" s="26">
+      <c r="C6" s="21">
+        <v>0</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="24">
         <f t="shared" ref="E6:E11" si="0">D6*C6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="26">
-        <v>0</v>
-      </c>
-      <c r="G6" s="26">
-        <v>0</v>
-      </c>
-      <c r="H6" s="26">
+      <c r="F6" s="24">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
         <f t="shared" ref="H6:H11" si="1">C6*(G6-F6)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="26">
-        <v>0</v>
-      </c>
-      <c r="J6" s="26">
+      <c r="I6" s="24">
+        <v>0</v>
+      </c>
+      <c r="J6" s="24">
         <f>C6*I6</f>
         <v>0</v>
       </c>
-      <c r="K6" s="26">
-        <v>0</v>
-      </c>
-      <c r="L6" s="26">
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
         <f t="shared" ref="L6" si="2">K6*J6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="24">
         <f>D6+G6+I6</f>
         <v>0</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="24">
         <f>E6+H6+J6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27">
+      <c r="B7" s="6"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28">
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="28">
+      <c r="I7" s="25"/>
+      <c r="J7" s="26">
         <f>C7*I7</f>
         <v>0</v>
       </c>
-      <c r="K7" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="28">
+      <c r="K7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="26">
         <f t="shared" ref="M7:M15" si="3">D7+G7+I7</f>
         <v>0</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="26">
         <f t="shared" ref="N7:N15" si="4">E7+H7+J7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20">
+      <c r="B8" s="8"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20">
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20">
+      <c r="I8" s="18"/>
+      <c r="J8" s="18">
         <f t="shared" ref="J8:J15" si="5">C8*I8</f>
         <v>0</v>
       </c>
-      <c r="K8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="20">
+      <c r="K8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27">
+      <c r="B9" s="6"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="28">
+      <c r="I9" s="25"/>
+      <c r="J9" s="26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K9" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="28">
+      <c r="K9" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="26">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20">
+      <c r="B10" s="8"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20">
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20">
+      <c r="I10" s="18"/>
+      <c r="J10" s="18">
         <f>C10*I10</f>
         <v>0</v>
       </c>
-      <c r="K10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" s="20">
+      <c r="K10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>6</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27">
+      <c r="B11" s="6"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28">
+      <c r="I11" s="25"/>
+      <c r="J11" s="26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K11" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="28">
+      <c r="K11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="26">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20">
+      <c r="B12" s="8"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18">
         <f t="shared" ref="E12:E15" si="6">D12*C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20">
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18">
         <f t="shared" ref="H12:H15" si="7">C12*(G12-F12)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20">
+      <c r="I12" s="18"/>
+      <c r="J12" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="20">
+      <c r="K12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N12" s="20">
+      <c r="N12" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>8</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27">
+      <c r="B13" s="6"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26">
         <f>C13*(G13-F13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28">
+      <c r="I13" s="25"/>
+      <c r="J13" s="26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K13" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="M13" s="28">
+      <c r="K13" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="26">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20">
+      <c r="B14" s="8"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20">
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18">
         <f>C14*(G14-F14)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20">
+      <c r="I14" s="18"/>
+      <c r="J14" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="20">
+      <c r="K14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
+      <c r="A15" s="9">
         <v>10</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30">
+      <c r="B15" s="10"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31">
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31">
+      <c r="I15" s="28"/>
+      <c r="J15" s="29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K15" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="M15" s="31">
+      <c r="K15" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="41" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="18">
+      <c r="C16" s="69"/>
+      <c r="D16" s="16">
         <f t="shared" ref="D16:N16" si="8">SUM(D5:D15)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="16">
         <f>SUM(F6:F15)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -1622,711 +1642,711 @@
       <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="23">
-        <v>0</v>
-      </c>
-      <c r="D19" s="17">
-        <v>0</v>
-      </c>
-      <c r="E19" s="17">
-        <f t="shared" ref="E19:E28" si="9">D19*C19</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="17">
-        <v>0</v>
-      </c>
-      <c r="G19" s="17">
-        <v>0</v>
-      </c>
-      <c r="H19" s="17">
-        <f t="shared" ref="H19:H28" si="10">G19*E19</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="17">
-        <v>0</v>
-      </c>
-      <c r="J19" s="17">
-        <f t="shared" ref="J19:J28" si="11">I19*H19</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="17">
-        <v>0</v>
-      </c>
-      <c r="L19" s="17">
-        <f t="shared" ref="L19" si="12">K19*J19</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="17">
-        <f t="shared" ref="M19:M28" si="13">D19+G19+I19</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="17">
-        <f t="shared" ref="N19" si="14">E19+H19+J19+L19</f>
+      <c r="C19" s="21">
+        <v>0</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15">
+        <f>D19*C19</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="15">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15">
+        <f>G19*C19</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15">
+        <f>I19*C19</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="15">
+        <v>0</v>
+      </c>
+      <c r="L19" s="15">
+        <f t="shared" ref="L19" si="9">K19*J19</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="15">
+        <f>D19+G19+I19</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="15">
+        <f t="shared" ref="N19" si="10">E19+H19+J19+L19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>2</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19">
-        <f>G20*E20</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19">
+      <c r="B20" s="6"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17">
+        <f>D20*C20</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17">
+        <f>G20*C20</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17">
+        <f>I20*C20</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" s="17">
+        <f>D20+G20+I20</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="17">
+        <f>E20+H20+J20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>3</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18">
+        <f>D21*C21</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
+        <f>G21*C21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
+        <f>I21*C21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="18">
+        <f t="shared" ref="M19:M28" si="11">D21+G21+I21</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="18">
+        <f t="shared" ref="N21:N28" si="12">E21+H21+J21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>4</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17">
+        <f>D22*C22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
+        <f>G22*C22</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
+        <f>I22*H22</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="17">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K20" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="M20" s="19">
+      <c r="N22" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>5</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18">
+        <f t="shared" ref="E19:E28" si="13">D23*C23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
+        <f>G23*C23</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18">
+        <f>I23*C23</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>6</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="N20" s="19">
-        <f>E20+H20+J20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>3</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17">
+        <f>G24*C24</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
+        <f>I24*C24</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24" s="17">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K21" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="20">
+      <c r="N24" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>7</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="N21" s="20">
-        <f t="shared" ref="N21:N28" si="15">E21+H21+J21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>4</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19">
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18">
+        <f>G25*C25</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18">
+        <f>I25*C25</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M25" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K22" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="M22" s="19">
+      <c r="N25" s="18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>8</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="N22" s="19">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>5</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20">
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17">
+        <f>G26*C26</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17">
+        <f>I26*C26</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M26" s="17">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M23" s="20">
+      <c r="N26" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>9</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="N23" s="20">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>6</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19">
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18">
+        <f>G27*C27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18">
+        <f>I27*C27</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M27" s="18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="M24" s="19">
+      <c r="N27" s="18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>10</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="N24" s="19">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>7</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20">
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19">
+        <f>G28*C28</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19">
+        <f>I28*C28</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M28" s="19">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K25" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M25" s="20">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="20">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>8</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="M26" s="19">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="19">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="N28" s="19">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M27" s="20">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="20">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
-        <v>10</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="M28" s="21">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="21">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="14">
-        <f t="shared" ref="D29:N29" si="16">SUM(D18:D28)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="14">
+      <c r="C29" s="69"/>
+      <c r="D29" s="12">
+        <f t="shared" ref="D29:N29" si="14">SUM(D18:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="12">
         <f>SUM(F19:F28)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="14">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N29" s="14">
-        <f t="shared" si="16"/>
+      <c r="G29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="12">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="73"/>
+      <c r="M31" s="73"/>
+      <c r="N31" s="73"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>1</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20">
-        <f t="shared" ref="E32:E35" si="17">D32*C32</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20">
-        <f t="shared" ref="H32:H35" si="18">G32*E32</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20">
-        <f t="shared" ref="J32:J35" si="19">I32*H32</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M32" s="20">
-        <f t="shared" ref="M32:M35" si="20">D32+G32+I32</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="20">
-        <f t="shared" ref="N32:N35" si="21">E32+H32+J32</f>
+      <c r="C32" s="83"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18">
+        <f>D32*C32</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18">
+        <f>G32*C32</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18">
+        <f>I32*C32</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M32" s="18">
+        <f t="shared" ref="M32:M35" si="15">D32+G32+I32</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="18">
+        <f t="shared" ref="N32:N35" si="16">E32+H32+J32</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="A33" s="5">
         <v>2</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19">
+      <c r="B33" s="6"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17">
+        <f t="shared" ref="E32:E35" si="17">D33*C33</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17">
+        <f>G33*C33</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17">
+        <f>I33*C33</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M33" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="17">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>3</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19">
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18">
+        <f>G34*C34</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18">
+        <f>I34*C34</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="18">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="18">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>4</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17">
+        <f>G35*C35</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17">
+        <f>I35*C35</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M35" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="17">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="67"/>
+      <c r="D36" s="32">
+        <f t="shared" ref="D36:N36" si="18">SUM(D31:D35)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="32">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="M33" s="19">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="19">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
-        <v>3</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20">
+      <c r="F36" s="32">
+        <f>SUM(F32:F35)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="32">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M34" s="20">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="20">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6">
+      <c r="H36" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+    </row>
+    <row r="39" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="61"/>
+      <c r="B39" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L35" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="M35" s="19">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="19">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50">
-        <f t="shared" ref="D36:N36" si="22">SUM(D31:D35)</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="50">
-        <f>SUM(F32:F35)</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="K36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="50">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
-    </row>
-    <row r="39" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="37" t="s">
+      <c r="E39" s="61"/>
+      <c r="F39" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40" t="s">
+      <c r="G39" s="63"/>
+      <c r="H39" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="40"/>
-      <c r="J39" s="35" t="s">
+      <c r="I39" s="60"/>
+      <c r="J39" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="K39" s="35"/>
+      <c r="K39" s="61"/>
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="2" t="s">
         <v>2</v>
       </c>
@@ -2353,389 +2373,382 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="77" t="s">
+      <c r="A41" s="54" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="55">
+      <c r="C41" s="76">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D41" s="24">
         <f>D29-D19</f>
         <v>0</v>
       </c>
-      <c r="E41" s="26">
+      <c r="E41" s="24">
         <f>D41*C41</f>
         <v>0</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F41" s="24">
         <f>G29-G19</f>
         <v>0</v>
       </c>
-      <c r="G41" s="26">
+      <c r="G41" s="24">
         <f>F41*C41</f>
         <v>0</v>
       </c>
-      <c r="H41" s="56">
-        <v>0</v>
-      </c>
-      <c r="I41" s="56">
+      <c r="H41" s="37">
+        <v>0</v>
+      </c>
+      <c r="I41" s="37">
         <f>H41*C41</f>
         <v>0</v>
       </c>
-      <c r="J41" s="26">
+      <c r="J41" s="24">
         <f>H41+F41+D41</f>
         <v>0</v>
       </c>
-      <c r="K41" s="26">
+      <c r="K41" s="24">
         <f>J41*C41</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="78" t="s">
+      <c r="A42" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="58">
+      <c r="C42" s="77">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D42" s="59">
+      <c r="D42" s="39">
         <f>D36</f>
         <v>0</v>
       </c>
-      <c r="E42" s="59">
+      <c r="E42" s="39">
         <f>D42*C42</f>
         <v>0</v>
       </c>
-      <c r="F42" s="59">
+      <c r="F42" s="39">
         <f>G36</f>
         <v>0</v>
       </c>
-      <c r="G42" s="59">
+      <c r="G42" s="39">
         <f>F42*C42</f>
         <v>0</v>
       </c>
-      <c r="H42" s="60">
-        <v>0</v>
-      </c>
-      <c r="I42" s="60">
+      <c r="H42" s="40">
+        <v>0</v>
+      </c>
+      <c r="I42" s="40">
         <f>H42*C42</f>
         <v>0</v>
       </c>
-      <c r="J42" s="59">
+      <c r="J42" s="39">
         <f>H42+F42+D42</f>
         <v>0</v>
       </c>
-      <c r="K42" s="59">
+      <c r="K42" s="39">
         <f>J42*C42</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72" t="s">
+      <c r="A43" s="48"/>
+      <c r="B43" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73">
+      <c r="C43" s="78"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50">
         <f>SUM(E41:E42)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="73"/>
-      <c r="G43" s="73">
+      <c r="F43" s="50"/>
+      <c r="G43" s="50">
         <f>SUM(G41:G42)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="73"/>
-      <c r="I43" s="73">
+      <c r="H43" s="50"/>
+      <c r="I43" s="50">
         <f>SUM(I41:I42)</f>
         <v>0</v>
       </c>
-      <c r="J43" s="73"/>
-      <c r="K43" s="73">
+      <c r="J43" s="50"/>
+      <c r="K43" s="50">
         <f>SUM(K41:K42)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J44" s="54"/>
+      <c r="C44" s="1"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="79" t="s">
+      <c r="A45" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="62">
+      <c r="C45" s="79">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D45" s="63">
+      <c r="D45" s="42">
         <f>D29-D19</f>
         <v>0</v>
       </c>
-      <c r="E45" s="63">
+      <c r="E45" s="42">
         <f>D45*C45</f>
         <v>0</v>
       </c>
-      <c r="F45" s="63">
+      <c r="F45" s="42">
         <f>G29-G19</f>
         <v>0</v>
       </c>
-      <c r="G45" s="63">
+      <c r="G45" s="42">
         <f>F45*C45</f>
         <v>0</v>
       </c>
-      <c r="H45" s="63">
+      <c r="H45" s="42">
         <f>K29-K19</f>
         <v>0</v>
       </c>
-      <c r="I45" s="63">
+      <c r="I45" s="42">
         <f>H45*C45</f>
         <v>0</v>
       </c>
-      <c r="J45" s="63">
+      <c r="J45" s="42">
         <f>H45+F45+D45</f>
         <v>0</v>
       </c>
-      <c r="K45" s="63">
+      <c r="K45" s="42">
         <f>J45*C45</f>
         <v>0</v>
       </c>
-      <c r="M45" s="54"/>
+      <c r="M45" s="36"/>
     </row>
     <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="80" t="s">
+      <c r="A46" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="65">
+      <c r="C46" s="80">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D46" s="66">
+      <c r="D46" s="44">
         <f>D36</f>
         <v>0</v>
       </c>
-      <c r="E46" s="66">
+      <c r="E46" s="44">
         <f>D46*C46</f>
         <v>0</v>
       </c>
-      <c r="F46" s="66">
+      <c r="F46" s="44">
         <f>G36</f>
         <v>0</v>
       </c>
-      <c r="G46" s="66">
+      <c r="G46" s="44">
         <f>F46*C46</f>
         <v>0</v>
       </c>
-      <c r="H46" s="66">
+      <c r="H46" s="44">
         <f>K36</f>
         <v>0</v>
       </c>
-      <c r="I46" s="66">
+      <c r="I46" s="44">
         <f>H46*C46</f>
         <v>0</v>
       </c>
-      <c r="J46" s="66">
+      <c r="J46" s="44">
         <f>H46+F46+D46</f>
         <v>0</v>
       </c>
-      <c r="K46" s="66">
+      <c r="K46" s="44">
         <f>J46*C46</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74"/>
-      <c r="B47" s="75" t="s">
+      <c r="A47" s="51"/>
+      <c r="B47" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="75"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="76">
+      <c r="C47" s="81"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53">
         <f>SUM(E45:E46)</f>
         <v>0</v>
       </c>
-      <c r="F47" s="76"/>
-      <c r="G47" s="76">
+      <c r="F47" s="53"/>
+      <c r="G47" s="53">
         <f>SUM(G45:G46)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="76"/>
-      <c r="I47" s="76">
+      <c r="H47" s="53"/>
+      <c r="I47" s="53">
         <f>SUM(I45:I46)</f>
         <v>0</v>
       </c>
-      <c r="J47" s="76"/>
-      <c r="K47" s="76">
+      <c r="J47" s="53"/>
+      <c r="K47" s="53">
         <f>SUM(K45:K46)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="N47" s="36"/>
+    </row>
+    <row r="48" spans="1:14" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="1"/>
+    </row>
     <row r="49" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="67" t="s">
+      <c r="B49" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="68">
+      <c r="C49" s="82">
         <v>0.01</v>
       </c>
-      <c r="D49" s="69">
+      <c r="D49" s="46">
         <f>D16-D6</f>
         <v>0</v>
       </c>
-      <c r="E49" s="69">
+      <c r="E49" s="46">
         <f>D49*C49</f>
         <v>0</v>
       </c>
-      <c r="F49" s="69">
+      <c r="F49" s="46">
         <f>G16-G6</f>
         <v>0</v>
       </c>
-      <c r="G49" s="69">
+      <c r="G49" s="46">
         <f>F49*C49</f>
         <v>0</v>
       </c>
-      <c r="H49" s="69">
+      <c r="H49" s="46">
         <f>K16-K6</f>
         <v>0</v>
       </c>
-      <c r="I49" s="69">
+      <c r="I49" s="46">
         <f>H49*C49</f>
         <v>0</v>
       </c>
-      <c r="J49" s="69">
+      <c r="J49" s="46">
         <f>H49+F49+D49</f>
         <v>0</v>
       </c>
-      <c r="K49" s="69">
+      <c r="K49" s="46">
         <f>J49*C49</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="74"/>
-      <c r="B50" s="75" t="s">
+      <c r="A50" s="51"/>
+      <c r="B50" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="75"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="76">
+      <c r="C50" s="81"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53">
         <f>SUM(E48:E49)</f>
         <v>0</v>
       </c>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76">
+      <c r="F50" s="53"/>
+      <c r="G50" s="53">
         <f>SUM(G48:G49)</f>
         <v>0</v>
       </c>
-      <c r="H50" s="76"/>
-      <c r="I50" s="76">
+      <c r="H50" s="53"/>
+      <c r="I50" s="53">
         <f>SUM(I48:I49)</f>
         <v>0</v>
       </c>
-      <c r="J50" s="76"/>
-      <c r="K50" s="76">
+      <c r="J50" s="53"/>
+      <c r="K50" s="53">
         <f>SUM(K48:K49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:11" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="1"/>
+    </row>
     <row r="52" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="82" t="s">
+      <c r="A52" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="67" t="s">
+      <c r="B52" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="68">
+      <c r="C52" s="82">
         <v>0.02</v>
       </c>
-      <c r="D52" s="69">
+      <c r="D52" s="46">
         <f>D16-D6</f>
         <v>0</v>
       </c>
-      <c r="E52" s="69">
+      <c r="E52" s="46">
         <f>D52*C52</f>
         <v>0</v>
       </c>
-      <c r="F52" s="69">
+      <c r="F52" s="46">
         <f>G16-G6</f>
         <v>0</v>
       </c>
-      <c r="G52" s="69">
+      <c r="G52" s="46">
         <f>F52*C52</f>
         <v>0</v>
       </c>
-      <c r="H52" s="70">
-        <v>0</v>
-      </c>
-      <c r="I52" s="70">
+      <c r="H52" s="47">
+        <v>0</v>
+      </c>
+      <c r="I52" s="47">
         <f>H52*C52</f>
         <v>0</v>
       </c>
-      <c r="J52" s="69">
+      <c r="J52" s="46">
         <f>H52+F52+D52</f>
         <v>0</v>
       </c>
-      <c r="K52" s="69">
+      <c r="K52" s="46">
         <f>J52*C52</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="74"/>
-      <c r="B53" s="75" t="s">
+      <c r="A53" s="51"/>
+      <c r="B53" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="75"/>
-      <c r="D53" s="76"/>
-      <c r="E53" s="76">
+      <c r="C53" s="81"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53">
         <f>SUM(E51:E52)</f>
         <v>0</v>
       </c>
-      <c r="F53" s="76"/>
-      <c r="G53" s="76">
+      <c r="F53" s="53"/>
+      <c r="G53" s="53">
         <f>SUM(G51:G52)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="76"/>
-      <c r="I53" s="76">
+      <c r="H53" s="53"/>
+      <c r="I53" s="53">
         <f>SUM(I51:I52)</f>
         <v>0</v>
       </c>
-      <c r="J53" s="76"/>
-      <c r="K53" s="76">
+      <c r="J53" s="53"/>
+      <c r="K53" s="53">
         <f>SUM(K51:K52)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A5:N5"/>
-    <mergeCell ref="A18:N18"/>
-    <mergeCell ref="A31:N31"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A3:A4"/>
@@ -2745,6 +2758,19 @@
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A5:N5"/>
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="A31:N31"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>